<commit_message>
Test upload of files without any edits
</commit_message>
<xml_diff>
--- a/data/demand_6periods.xlsx
+++ b/data/demand_6periods.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chriska\Documents\01_modeling\Programming Sandbox\xpress\PMM\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matti\Documents\pmm\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="demand">Sheet1!$A$1:$I$18</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,20 +352,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G37"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -376,7 +376,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -387,7 +387,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -398,7 +398,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -409,7 +409,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -420,7 +420,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -431,7 +431,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>